<commit_message>
Updated positions and bills codebooks, readme
</commit_message>
<xml_diff>
--- a/codebook/bills_codebook.xlsx
+++ b/codebook/bills_codebook.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ejhall2/Desktop/Projects/chorus_data/info/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ejhall2/Desktop/Projects/CHORUS/chorus_data/codebook/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAA5ED58-DE81-7C42-B8F0-75E53B395756}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08E5FA6F-CFC6-4340-84F5-B7DA605104C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="88">
   <si>
     <t>Variable</t>
   </si>
@@ -240,9 +240,6 @@
     <t>date_overlap_jaccard</t>
   </si>
   <si>
-    <t>0.896774193548387</t>
-  </si>
-  <si>
     <t>A measure of how well the date range for this bill in LegiScan overlapped with the date range in StateNet</t>
   </si>
   <si>
@@ -253,9 +250,6 @@
   </si>
   <si>
     <t>title_overlap_jaccard</t>
-  </si>
-  <si>
-    <t>0.5217391304347826</t>
   </si>
   <si>
     <t>A measure of how well the title for this bill in LegiScan overlapped with the title in StateNet</t>
@@ -313,18 +307,21 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -595,7 +592,7 @@
   <dimension ref="A1:G1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1074,20 +1071,20 @@
       <c r="B24" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="C24" s="2" t="s">
+      <c r="C24" s="2">
+        <v>0.89700000000000002</v>
+      </c>
+      <c r="D24" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="D24" s="2" t="s">
+      <c r="E24" s="2" t="s">
         <v>72</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>73</v>
       </c>
       <c r="F24" s="2" t="s">
         <v>50</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1095,22 +1092,22 @@
         <v>23</v>
       </c>
       <c r="B25" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C25" s="2">
+        <v>0.52300000000000002</v>
+      </c>
+      <c r="D25" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="C25" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>77</v>
-      </c>
       <c r="E25" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F25" s="2" t="s">
         <v>50</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1118,13 +1115,13 @@
         <v>24</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E26" s="2" t="s">
         <v>13</v>
@@ -1138,13 +1135,13 @@
         <v>25</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E27" s="2" t="s">
         <v>13</v>
@@ -1158,13 +1155,13 @@
         <v>26</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E28" s="2" t="s">
         <v>13</v>
@@ -1178,13 +1175,13 @@
         <v>27</v>
       </c>
       <c r="B29" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="D29" s="3" t="s">
         <v>84</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="D29" s="3" t="s">
-        <v>86</v>
       </c>
       <c r="E29" s="2" t="s">
         <v>13</v>

</xml_diff>